<commit_message>
add save file  part
</commit_message>
<xml_diff>
--- a/Documents/进度安排（4月22-4月28）.xlsx
+++ b/Documents/进度安排（4月22-4月28）.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jskyhuang\workspace\unity\Unity.ExtendEditor\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B393042-1821-4661-8DFB-6FF2E28482AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E453D5C-6A3C-46C9-9C50-EB376A7AD650}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="7185" xr2:uid="{05249081-CE36-444F-9005-18DB7237BD5F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23220" windowHeight="3270" xr2:uid="{05249081-CE36-444F-9005-18DB7237BD5F}"/>
   </bookViews>
   <sheets>
     <sheet name="时间计划表" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,39 +119,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -163,18 +137,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -193,20 +161,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="差" xfId="2" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -521,7 +481,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -573,7 +533,6 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -585,7 +544,7 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -696,7 +655,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>43582</v>
       </c>
       <c r="B10" s="3">
@@ -717,7 +676,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="3">
         <v>0.52083333333333337</v>
       </c>
@@ -736,7 +695,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
@@ -748,7 +707,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
@@ -760,7 +719,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="3">
         <v>0.77083333333333337</v>
       </c>
@@ -773,7 +732,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>43583</v>
       </c>
       <c r="B15" s="3">
@@ -788,7 +747,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="3">
         <v>0.52083333333333337</v>
       </c>
@@ -801,7 +760,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>0.77083333333333337</v>
       </c>

</xml_diff>